<commit_message>
added forecast for multi steps
</commit_message>
<xml_diff>
--- a/Predictions/my_last_24.xlsx
+++ b/Predictions/my_last_24.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\sulith\LSTM\LSTM_Wind_assignment\Predictions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7A7AADFB-FC42-4F96-AC76-49D85E955D6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{462C7401-BBF7-4284-819B-5A2E07A107B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{226C3F7D-FFBB-4DBE-8E87-AFDD51D7A649}"/>
   </bookViews>
@@ -153,7 +153,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -652,11 +652,9 @@
     <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1039,10 +1037,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F6A4D59-19D9-4241-A06E-A05E27A5E9C2}">
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A37"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1311,7 +1309,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+      <c r="A14" t="s">
         <v>18</v>
       </c>
       <c r="B14">
@@ -1331,7 +1329,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+      <c r="A15" t="s">
         <v>19</v>
       </c>
       <c r="B15">
@@ -1351,7 +1349,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+      <c r="A16" t="s">
         <v>20</v>
       </c>
       <c r="B16">
@@ -1371,7 +1369,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+      <c r="A17" t="s">
         <v>21</v>
       </c>
       <c r="B17">
@@ -1391,7 +1389,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+      <c r="A18" t="s">
         <v>22</v>
       </c>
       <c r="B18">
@@ -1411,7 +1409,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+      <c r="A19" t="s">
         <v>23</v>
       </c>
       <c r="B19">
@@ -1431,7 +1429,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+      <c r="A20" t="s">
         <v>24</v>
       </c>
       <c r="B20">
@@ -1451,7 +1449,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+      <c r="A21" t="s">
         <v>25</v>
       </c>
       <c r="B21">
@@ -1471,7 +1469,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+      <c r="A22" t="s">
         <v>26</v>
       </c>
       <c r="B22">
@@ -1491,7 +1489,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
+      <c r="A23" t="s">
         <v>27</v>
       </c>
       <c r="B23">
@@ -1511,7 +1509,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
+      <c r="A24" t="s">
         <v>28</v>
       </c>
       <c r="B24">
@@ -1531,7 +1529,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
+      <c r="A25" t="s">
         <v>29</v>
       </c>
       <c r="B25">
@@ -1551,7 +1549,7 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
+      <c r="A26" t="s">
         <v>30</v>
       </c>
       <c r="B26">
@@ -1571,7 +1569,7 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
+      <c r="A27" t="s">
         <v>31</v>
       </c>
       <c r="B27">
@@ -1591,7 +1589,7 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
+      <c r="A28" t="s">
         <v>32</v>
       </c>
       <c r="B28">
@@ -1611,7 +1609,7 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
+      <c r="A29" t="s">
         <v>33</v>
       </c>
       <c r="B29">
@@ -1631,7 +1629,7 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
+      <c r="A30" t="s">
         <v>34</v>
       </c>
       <c r="B30">
@@ -1651,7 +1649,7 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
+      <c r="A31" t="s">
         <v>35</v>
       </c>
       <c r="B31">
@@ -1671,7 +1669,7 @@
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="3" t="s">
+      <c r="A32" t="s">
         <v>36</v>
       </c>
       <c r="B32">
@@ -1691,7 +1689,7 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="3" t="s">
+      <c r="A33" t="s">
         <v>37</v>
       </c>
       <c r="B33">
@@ -1711,7 +1709,7 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="3" t="s">
+      <c r="A34" t="s">
         <v>38</v>
       </c>
       <c r="B34">
@@ -1731,7 +1729,7 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="3" t="s">
+      <c r="A35" t="s">
         <v>39</v>
       </c>
       <c r="B35">
@@ -1751,7 +1749,7 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="3" t="s">
+      <c r="A36" t="s">
         <v>40</v>
       </c>
       <c r="B36">
@@ -1771,7 +1769,7 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="3" t="s">
+      <c r="A37" t="s">
         <v>41</v>
       </c>
       <c r="B37">
@@ -1789,27 +1787,10 @@
       <c r="F37">
         <v>0.68926751799999997</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="3"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="3"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="3"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="3"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" s="3"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>